<commit_message>
update all the test case by max_uncolored_rows 85%
</commit_message>
<xml_diff>
--- a/xjh/TEST/F4/postprocess.xlsx
+++ b/xjh/TEST/F4/postprocess.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xjh/thesis/xjh/TEST/F4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E52396-C323-B14D-B957-672664DE65AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0B0E01-D216-DB46-9168-D4F05C724135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E813E3D2-8B92-5C49-8DD6-185F646B6F3F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{E813E3D2-8B92-5C49-8DD6-185F646B6F3F}"/>
   </bookViews>
   <sheets>
-    <sheet name="coarse_CPU" sheetId="1" r:id="rId1"/>
-    <sheet name="ILU0_GPU_coarse" sheetId="4" r:id="rId2"/>
-    <sheet name="ILU1_GPU_coarse" sheetId="5" r:id="rId3"/>
+    <sheet name="CPU" sheetId="1" r:id="rId1"/>
+    <sheet name="ILU0_GPU" sheetId="4" r:id="rId2"/>
+    <sheet name="ILU1_GPU" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="21">
   <si>
     <t>LU分解耗时</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t xml:space="preserve">|res|/|res0| </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Smoother used </t>
   </si>
 </sst>
 </file>
@@ -574,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BEE77C-FC9B-2A4B-B70C-ACB86D236C97}">
   <dimension ref="A1:BP256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
@@ -8837,8 +8834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60AECBB-FA79-814B-BF8F-04A58F7DEA5D}">
   <dimension ref="A1:AA137"/>
   <sheetViews>
-    <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="M53" sqref="M3:M53"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8921,25 +8918,25 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>1.7499299999999999E-2</v>
+        <v>1.4424599999999999E-2</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3">
-        <v>1.0221399999999999E-3</v>
+        <v>8.1779200000000002E-4</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="G3">
-        <v>1.2104800000000001E-2</v>
+        <v>8.2929300000000004E-3</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I3">
-        <v>5.6350699999999998E-3</v>
+        <v>4.6602600000000003E-3</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
@@ -8951,13 +8948,13 @@
         <v>16</v>
       </c>
       <c r="M3" s="4">
-        <v>9.618789E-5</v>
+        <v>9.9274349999999996E-5</v>
       </c>
       <c r="N3" t="s">
         <v>17</v>
       </c>
       <c r="O3">
-        <v>0.72899999999999998</v>
+        <v>1.0940000000000001</v>
       </c>
       <c r="T3" s="4"/>
     </row>
@@ -8969,25 +8966,25 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>1.83952E-2</v>
+        <v>1.2215699999999999E-2</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4">
-        <v>1.02768E-3</v>
+        <v>8.3091199999999995E-4</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4">
-        <v>9.8242899999999994E-3</v>
+        <v>8.2805099999999996E-3</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I4">
-        <v>5.62278E-3</v>
+        <v>4.6530599999999997E-3</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -8999,13 +8996,13 @@
         <v>16</v>
       </c>
       <c r="M4" s="4">
-        <v>8.1659919999999995E-5</v>
+        <v>9.4235940000000006E-5</v>
       </c>
       <c r="N4" t="s">
         <v>17</v>
       </c>
       <c r="O4">
-        <v>0.72899999999999998</v>
+        <v>1.0940000000000001</v>
       </c>
       <c r="T4" s="4"/>
     </row>
@@ -9017,43 +9014,43 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1.7045600000000001E-2</v>
+        <v>1.34518E-2</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5">
-        <v>1.0249600000000001E-3</v>
+        <v>8.2543999999999998E-4</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="G5">
-        <v>9.8407700000000004E-3</v>
+        <v>9.6057E-3</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I5">
-        <v>5.6391699999999998E-3</v>
+        <v>5.34016E-3</v>
       </c>
       <c r="J5" t="s">
         <v>15</v>
       </c>
       <c r="K5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L5" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="4">
-        <v>8.6278200000000003E-5</v>
+        <v>2.4801130000000001E-5</v>
       </c>
       <c r="N5" t="s">
         <v>17</v>
       </c>
       <c r="O5">
-        <v>0.72899999999999998</v>
+        <v>1.0940000000000001</v>
       </c>
       <c r="T5" s="4"/>
     </row>
@@ -9065,25 +9062,25 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.303454</v>
+        <v>0.310222</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6">
-        <v>3.9567100000000001E-2</v>
+        <v>3.3448899999999997E-2</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6">
-        <v>0.219143</v>
+        <v>0.227437</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I6">
-        <v>0.13144400000000001</v>
+        <v>0.123613</v>
       </c>
       <c r="J6" t="s">
         <v>15</v>
@@ -9095,13 +9092,13 @@
         <v>16</v>
       </c>
       <c r="M6" s="4">
-        <v>7.5098750000000003E-5</v>
+        <v>8.1346479999999996E-5</v>
       </c>
       <c r="N6" t="s">
         <v>17</v>
       </c>
       <c r="O6">
-        <v>6.72</v>
+        <v>7.085</v>
       </c>
       <c r="T6" s="4"/>
     </row>
@@ -9113,25 +9110,25 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.32240000000000002</v>
+        <v>0.29269200000000001</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7">
-        <v>3.94995E-2</v>
+        <v>3.34215E-2</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
       <c r="G7">
-        <v>0.22603999999999999</v>
+        <v>0.212339</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I7">
-        <v>0.13145999999999999</v>
+        <v>0.12359100000000001</v>
       </c>
       <c r="J7" t="s">
         <v>15</v>
@@ -9143,13 +9140,13 @@
         <v>16</v>
       </c>
       <c r="M7" s="4">
-        <v>6.7063259999999996E-5</v>
+        <v>7.2408109999999996E-5</v>
       </c>
       <c r="N7" t="s">
         <v>17</v>
       </c>
       <c r="O7">
-        <v>6.72</v>
+        <v>7.085</v>
       </c>
       <c r="T7" s="4"/>
     </row>
@@ -9161,25 +9158,25 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>0.302506</v>
+        <v>0.29517100000000002</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8">
-        <v>3.9391700000000002E-2</v>
+        <v>3.3342299999999998E-2</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8">
-        <v>0.21959000000000001</v>
+        <v>0.215252</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I8">
-        <v>0.13145799999999999</v>
+        <v>0.12361999999999999</v>
       </c>
       <c r="J8" t="s">
         <v>15</v>
@@ -9191,13 +9188,13 @@
         <v>16</v>
       </c>
       <c r="M8" s="4">
-        <v>5.5801000000000003E-5</v>
+        <v>5.9868419999999999E-5</v>
       </c>
       <c r="N8" t="s">
         <v>17</v>
       </c>
       <c r="O8">
-        <v>6.72</v>
+        <v>7.085</v>
       </c>
       <c r="T8" s="4"/>
     </row>
@@ -9209,25 +9206,25 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>0.30719000000000002</v>
+        <v>0.31284099999999998</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
       <c r="E9">
-        <v>3.9474500000000003E-2</v>
+        <v>3.3341299999999997E-2</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
       <c r="G9">
-        <v>0.22311500000000001</v>
+        <v>0.229598</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I9">
-        <v>0.131435</v>
+        <v>0.123603</v>
       </c>
       <c r="J9" t="s">
         <v>15</v>
@@ -9239,13 +9236,13 @@
         <v>16</v>
       </c>
       <c r="M9" s="4">
-        <v>4.5799759999999999E-5</v>
+        <v>4.8902210000000002E-5</v>
       </c>
       <c r="N9" t="s">
         <v>17</v>
       </c>
       <c r="O9">
-        <v>6.72</v>
+        <v>7.085</v>
       </c>
       <c r="T9" s="4"/>
     </row>
@@ -9257,25 +9254,25 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>0.30339700000000003</v>
+        <v>0.296684</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10">
-        <v>3.9577800000000003E-2</v>
+        <v>3.34186E-2</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
       <c r="G10">
-        <v>0.22201199999999999</v>
+        <v>0.220361</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I10">
-        <v>0.13145200000000001</v>
+        <v>0.12358</v>
       </c>
       <c r="J10" t="s">
         <v>15</v>
@@ -9287,13 +9284,13 @@
         <v>16</v>
       </c>
       <c r="M10" s="4">
-        <v>3.7827529999999999E-5</v>
+        <v>4.0402009999999998E-5</v>
       </c>
       <c r="N10" t="s">
         <v>17</v>
       </c>
       <c r="O10">
-        <v>6.72</v>
+        <v>7.085</v>
       </c>
       <c r="T10" s="4"/>
     </row>
@@ -9305,25 +9302,25 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.30049500000000001</v>
+        <v>0.29525099999999999</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11">
-        <v>3.9559700000000003E-2</v>
+        <v>3.3401699999999999E-2</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11">
-        <v>0.21944900000000001</v>
+        <v>0.21701000000000001</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I11">
-        <v>0.131495</v>
+        <v>0.12361800000000001</v>
       </c>
       <c r="J11" t="s">
         <v>15</v>
@@ -9335,13 +9332,13 @@
         <v>16</v>
       </c>
       <c r="M11" s="4">
-        <v>3.1241700000000003E-5</v>
+        <v>3.3482249999999999E-5</v>
       </c>
       <c r="N11" t="s">
         <v>17</v>
       </c>
       <c r="O11">
-        <v>6.72</v>
+        <v>7.085</v>
       </c>
       <c r="T11" s="4"/>
     </row>
@@ -9353,43 +9350,43 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>0.275032</v>
+        <v>0.29782799999999998</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12">
-        <v>3.9464300000000001E-2</v>
+        <v>3.3350200000000003E-2</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
       <c r="G12">
-        <v>0.19293099999999999</v>
+        <v>0.218892</v>
       </c>
       <c r="H12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I12">
-        <v>0.115047</v>
+        <v>0.12363</v>
       </c>
       <c r="J12" t="s">
         <v>15</v>
       </c>
       <c r="K12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L12" t="s">
         <v>16</v>
       </c>
       <c r="M12" s="4">
-        <v>9.8837630000000006E-5</v>
+        <v>2.7450060000000001E-5</v>
       </c>
       <c r="N12" t="s">
         <v>17</v>
       </c>
       <c r="O12">
-        <v>6.6180000000000003</v>
+        <v>7.085</v>
       </c>
       <c r="T12" s="4"/>
     </row>
@@ -9401,25 +9398,25 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <v>0.28120899999999999</v>
+        <v>0.26882400000000001</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13">
-        <v>3.95222E-2</v>
+        <v>3.3431500000000003E-2</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13">
-        <v>0.191</v>
+        <v>0.18973300000000001</v>
       </c>
       <c r="H13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I13">
-        <v>0.115022</v>
+        <v>0.10817599999999999</v>
       </c>
       <c r="J13" t="s">
         <v>15</v>
@@ -9431,13 +9428,13 @@
         <v>16</v>
       </c>
       <c r="M13" s="4">
-        <v>8.2490059999999995E-5</v>
+        <v>8.6199350000000003E-5</v>
       </c>
       <c r="N13" t="s">
         <v>17</v>
       </c>
       <c r="O13">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T13" s="4"/>
     </row>
@@ -9449,25 +9446,25 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>0.27300400000000002</v>
+        <v>0.26436199999999999</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14">
-        <v>3.9503799999999999E-2</v>
+        <v>3.3335200000000002E-2</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
       </c>
       <c r="G14">
-        <v>0.18892600000000001</v>
+        <v>0.18509700000000001</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I14">
-        <v>0.115088</v>
+        <v>0.108149</v>
       </c>
       <c r="J14" t="s">
         <v>15</v>
@@ -9479,13 +9476,13 @@
         <v>16</v>
       </c>
       <c r="M14" s="4">
-        <v>6.9908779999999996E-5</v>
+        <v>7.3246080000000002E-5</v>
       </c>
       <c r="N14" t="s">
         <v>17</v>
       </c>
       <c r="O14">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T14" s="4"/>
     </row>
@@ -9497,25 +9494,25 @@
         <v>5</v>
       </c>
       <c r="C15">
-        <v>0.268183</v>
+        <v>0.25581399999999999</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15">
-        <v>3.9555699999999999E-2</v>
+        <v>3.3454600000000001E-2</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
       </c>
       <c r="G15">
-        <v>0.18757399999999999</v>
+        <v>0.18181700000000001</v>
       </c>
       <c r="H15" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I15">
-        <v>0.11505600000000001</v>
+        <v>0.108144</v>
       </c>
       <c r="J15" t="s">
         <v>15</v>
@@ -9527,13 +9524,13 @@
         <v>16</v>
       </c>
       <c r="M15" s="4">
-        <v>5.9863430000000002E-5</v>
+        <v>6.3754169999999998E-5</v>
       </c>
       <c r="N15" t="s">
         <v>17</v>
       </c>
       <c r="O15">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T15" s="4"/>
     </row>
@@ -9545,25 +9542,25 @@
         <v>5</v>
       </c>
       <c r="C16">
-        <v>0.279115</v>
+        <v>0.260295</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16">
-        <v>3.9495599999999999E-2</v>
+        <v>3.3433900000000003E-2</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
       </c>
       <c r="G16">
-        <v>0.193941</v>
+        <v>0.18625900000000001</v>
       </c>
       <c r="H16" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I16">
-        <v>0.11507199999999999</v>
+        <v>0.108164</v>
       </c>
       <c r="J16" t="s">
         <v>15</v>
@@ -9575,13 +9572,13 @@
         <v>16</v>
       </c>
       <c r="M16" s="4">
-        <v>5.171555E-5</v>
+        <v>5.656851E-5</v>
       </c>
       <c r="N16" t="s">
         <v>17</v>
       </c>
       <c r="O16">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T16" s="4"/>
     </row>
@@ -9593,25 +9590,25 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>0.27834100000000001</v>
+        <v>0.29067599999999999</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17">
-        <v>3.9565500000000003E-2</v>
+        <v>3.3388800000000003E-2</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
       <c r="G17">
-        <v>0.19361700000000001</v>
+        <v>0.19159699999999999</v>
       </c>
       <c r="H17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I17">
-        <v>0.115033</v>
+        <v>0.108152</v>
       </c>
       <c r="J17" t="s">
         <v>15</v>
@@ -9623,13 +9620,13 @@
         <v>16</v>
       </c>
       <c r="M17" s="4">
-        <v>4.522691E-5</v>
+        <v>5.1899459999999997E-5</v>
       </c>
       <c r="N17" t="s">
         <v>17</v>
       </c>
       <c r="O17">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T17" s="4"/>
     </row>
@@ -9641,25 +9638,25 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>0.27922599999999997</v>
+        <v>0.26966299999999999</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18">
-        <v>3.9479500000000001E-2</v>
+        <v>3.3451300000000003E-2</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
       </c>
       <c r="G18">
-        <v>0.192907</v>
+        <v>0.18631400000000001</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I18">
-        <v>0.115061</v>
+        <v>0.108149</v>
       </c>
       <c r="J18" t="s">
         <v>15</v>
@@ -9671,13 +9668,13 @@
         <v>16</v>
       </c>
       <c r="M18" s="4">
-        <v>4.0270579999999999E-5</v>
+        <v>4.9038349999999998E-5</v>
       </c>
       <c r="N18" t="s">
         <v>17</v>
       </c>
       <c r="O18">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T18" s="4"/>
     </row>
@@ -9689,25 +9686,25 @@
         <v>5</v>
       </c>
       <c r="C19">
-        <v>0.26947500000000002</v>
+        <v>0.28085199999999999</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19">
-        <v>3.95106E-2</v>
+        <v>3.3248600000000003E-2</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
       <c r="G19">
-        <v>0.18898100000000001</v>
+        <v>0.19597300000000001</v>
       </c>
       <c r="H19" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I19">
-        <v>0.115025</v>
+        <v>0.10814699999999999</v>
       </c>
       <c r="J19" t="s">
         <v>15</v>
@@ -9719,13 +9716,13 @@
         <v>16</v>
       </c>
       <c r="M19" s="4">
-        <v>3.7096240000000002E-5</v>
+        <v>4.7537229999999998E-5</v>
       </c>
       <c r="N19" t="s">
         <v>17</v>
       </c>
       <c r="O19">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T19" s="4"/>
     </row>
@@ -9737,25 +9734,25 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <v>0.276119</v>
+        <v>0.27649099999999999</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
       <c r="E20">
-        <v>3.9545999999999998E-2</v>
+        <v>3.3404799999999998E-2</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
       <c r="G20">
-        <v>0.18917400000000001</v>
+        <v>0.19925599999999999</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I20">
-        <v>0.115009</v>
+        <v>0.108164</v>
       </c>
       <c r="J20" t="s">
         <v>15</v>
@@ -9767,13 +9764,13 @@
         <v>16</v>
       </c>
       <c r="M20" s="4">
-        <v>3.4763949999999998E-5</v>
+        <v>4.6883269999999997E-5</v>
       </c>
       <c r="N20" t="s">
         <v>17</v>
       </c>
       <c r="O20">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T20" s="4"/>
     </row>
@@ -9785,25 +9782,25 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <v>0.268569</v>
+        <v>0.26714300000000002</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
       </c>
       <c r="E21">
-        <v>3.96713E-2</v>
+        <v>3.3300400000000001E-2</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21">
-        <v>0.187665</v>
+        <v>0.184779</v>
       </c>
       <c r="H21" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I21">
-        <v>0.115094</v>
+        <v>0.10814</v>
       </c>
       <c r="J21" t="s">
         <v>15</v>
@@ -9815,13 +9812,13 @@
         <v>16</v>
       </c>
       <c r="M21" s="4">
-        <v>3.3904430000000002E-5</v>
+        <v>4.7647440000000003E-5</v>
       </c>
       <c r="N21" t="s">
         <v>17</v>
       </c>
       <c r="O21">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T21" s="4"/>
     </row>
@@ -9833,25 +9830,25 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <v>0.28153099999999998</v>
+        <v>0.26848899999999998</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
       <c r="E22">
-        <v>3.9472899999999998E-2</v>
+        <v>3.3371999999999999E-2</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22">
-        <v>0.189777</v>
+        <v>0.18648899999999999</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I22">
-        <v>0.115012</v>
+        <v>0.108154</v>
       </c>
       <c r="J22" t="s">
         <v>15</v>
@@ -9863,13 +9860,13 @@
         <v>16</v>
       </c>
       <c r="M22" s="4">
-        <v>3.3717490000000003E-5</v>
+        <v>4.8506730000000003E-5</v>
       </c>
       <c r="N22" t="s">
         <v>17</v>
       </c>
       <c r="O22">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T22" s="4"/>
     </row>
@@ -9881,25 +9878,25 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <v>0.28974299999999997</v>
+        <v>0.27578000000000003</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23">
-        <v>3.94872E-2</v>
+        <v>3.3386800000000001E-2</v>
       </c>
       <c r="F23" t="s">
         <v>13</v>
       </c>
       <c r="G23">
-        <v>0.19846800000000001</v>
+        <v>0.190857</v>
       </c>
       <c r="H23" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I23">
-        <v>0.115024</v>
+        <v>0.108167</v>
       </c>
       <c r="J23" t="s">
         <v>15</v>
@@ -9911,13 +9908,13 @@
         <v>16</v>
       </c>
       <c r="M23" s="4">
-        <v>3.4507159999999998E-5</v>
+        <v>4.8784810000000002E-5</v>
       </c>
       <c r="N23" t="s">
         <v>17</v>
       </c>
       <c r="O23">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T23" s="4"/>
     </row>
@@ -9929,25 +9926,25 @@
         <v>5</v>
       </c>
       <c r="C24">
-        <v>0.27481299999999997</v>
+        <v>0.28048800000000002</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
       <c r="E24">
-        <v>3.9558099999999999E-2</v>
+        <v>3.3493500000000002E-2</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
       </c>
       <c r="G24">
-        <v>0.192722</v>
+        <v>0.186783</v>
       </c>
       <c r="H24" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I24">
-        <v>0.11501599999999999</v>
+        <v>0.108127</v>
       </c>
       <c r="J24" t="s">
         <v>15</v>
@@ -9959,13 +9956,13 @@
         <v>16</v>
       </c>
       <c r="M24" s="4">
-        <v>3.4656039999999998E-5</v>
+        <v>4.9379329999999999E-5</v>
       </c>
       <c r="N24" t="s">
         <v>17</v>
       </c>
       <c r="O24">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T24" s="4"/>
     </row>
@@ -9977,25 +9974,25 @@
         <v>5</v>
       </c>
       <c r="C25">
-        <v>0.27999299999999999</v>
+        <v>0.26094899999999999</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
       <c r="E25">
-        <v>3.9541800000000002E-2</v>
+        <v>3.3386199999999998E-2</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25">
-        <v>0.192298</v>
+        <v>0.18701499999999999</v>
       </c>
       <c r="H25" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I25">
-        <v>0.114995</v>
+        <v>0.108163</v>
       </c>
       <c r="J25" t="s">
         <v>15</v>
@@ -10007,13 +10004,13 @@
         <v>16</v>
       </c>
       <c r="M25" s="4">
-        <v>3.5285679999999999E-5</v>
+        <v>5.0594930000000001E-5</v>
       </c>
       <c r="N25" t="s">
         <v>17</v>
       </c>
       <c r="O25">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T25" s="4"/>
     </row>
@@ -10025,25 +10022,25 @@
         <v>5</v>
       </c>
       <c r="C26">
-        <v>0.27476</v>
+        <v>0.26991799999999999</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
       <c r="E26">
-        <v>3.9497999999999998E-2</v>
+        <v>3.33554E-2</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
       </c>
       <c r="G26">
-        <v>0.19406399999999999</v>
+        <v>0.191883</v>
       </c>
       <c r="H26" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I26">
-        <v>0.115009</v>
+        <v>0.10815900000000001</v>
       </c>
       <c r="J26" t="s">
         <v>15</v>
@@ -10055,13 +10052,13 @@
         <v>16</v>
       </c>
       <c r="M26" s="4">
-        <v>3.414404E-5</v>
+        <v>4.9484480000000002E-5</v>
       </c>
       <c r="N26" t="s">
         <v>17</v>
       </c>
       <c r="O26">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T26" s="4"/>
     </row>
@@ -10073,25 +10070,25 @@
         <v>5</v>
       </c>
       <c r="C27">
-        <v>0.29042400000000002</v>
+        <v>0.27044899999999999</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
       </c>
       <c r="E27">
-        <v>3.9417300000000002E-2</v>
+        <v>3.3426999999999998E-2</v>
       </c>
       <c r="F27" t="s">
         <v>13</v>
       </c>
       <c r="G27">
-        <v>0.193076</v>
+        <v>0.18942600000000001</v>
       </c>
       <c r="H27" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I27">
-        <v>0.11505899999999999</v>
+        <v>0.108167</v>
       </c>
       <c r="J27" t="s">
         <v>15</v>
@@ -10103,13 +10100,13 @@
         <v>16</v>
       </c>
       <c r="M27" s="4">
-        <v>3.3575170000000001E-5</v>
+        <v>4.9336969999999997E-5</v>
       </c>
       <c r="N27" t="s">
         <v>17</v>
       </c>
       <c r="O27">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T27" s="4"/>
     </row>
@@ -10121,25 +10118,25 @@
         <v>5</v>
       </c>
       <c r="C28">
-        <v>0.27539999999999998</v>
+        <v>0.27246999999999999</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
       </c>
       <c r="E28">
-        <v>3.9588499999999999E-2</v>
+        <v>3.3376099999999999E-2</v>
       </c>
       <c r="F28" t="s">
         <v>13</v>
       </c>
       <c r="G28">
-        <v>0.19314300000000001</v>
+        <v>0.19873499999999999</v>
       </c>
       <c r="H28" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I28">
-        <v>0.115041</v>
+        <v>0.108172</v>
       </c>
       <c r="J28" t="s">
         <v>15</v>
@@ -10151,13 +10148,13 @@
         <v>16</v>
       </c>
       <c r="M28" s="4">
-        <v>3.339363E-5</v>
+        <v>4.9871389999999998E-5</v>
       </c>
       <c r="N28" t="s">
         <v>17</v>
       </c>
       <c r="O28">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T28" s="4"/>
     </row>
@@ -10169,25 +10166,25 @@
         <v>5</v>
       </c>
       <c r="C29">
-        <v>0.28421999999999997</v>
+        <v>0.26072400000000001</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
       <c r="E29">
-        <v>3.9442199999999997E-2</v>
+        <v>3.3420100000000001E-2</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
       </c>
       <c r="G29">
-        <v>0.197911</v>
+        <v>0.18257100000000001</v>
       </c>
       <c r="H29" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I29">
-        <v>0.115018</v>
+        <v>0.108185</v>
       </c>
       <c r="J29" t="s">
         <v>15</v>
@@ -10199,13 +10196,13 @@
         <v>16</v>
       </c>
       <c r="M29" s="4">
-        <v>3.2791389999999998E-5</v>
+        <v>5.0087170000000002E-5</v>
       </c>
       <c r="N29" t="s">
         <v>17</v>
       </c>
       <c r="O29">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T29" s="4"/>
     </row>
@@ -10217,25 +10214,25 @@
         <v>5</v>
       </c>
       <c r="C30">
-        <v>0.27339000000000002</v>
+        <v>0.27704099999999998</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
       </c>
       <c r="E30">
-        <v>3.9499399999999997E-2</v>
+        <v>3.3327099999999998E-2</v>
       </c>
       <c r="F30" t="s">
         <v>13</v>
       </c>
       <c r="G30">
-        <v>0.18808800000000001</v>
+        <v>0.19538800000000001</v>
       </c>
       <c r="H30" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I30">
-        <v>0.11504200000000001</v>
+        <v>0.108149</v>
       </c>
       <c r="J30" t="s">
         <v>15</v>
@@ -10247,13 +10244,13 @@
         <v>16</v>
       </c>
       <c r="M30" s="4">
-        <v>3.1963540000000003E-5</v>
+        <v>5.0006129999999998E-5</v>
       </c>
       <c r="N30" t="s">
         <v>17</v>
       </c>
       <c r="O30">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T30" s="4"/>
     </row>
@@ -10265,25 +10262,25 @@
         <v>5</v>
       </c>
       <c r="C31">
-        <v>0.276416</v>
+        <v>0.27644800000000003</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31">
-        <v>3.9538999999999998E-2</v>
+        <v>3.3396000000000002E-2</v>
       </c>
       <c r="F31" t="s">
         <v>13</v>
       </c>
       <c r="G31">
-        <v>0.19448099999999999</v>
+        <v>0.19103800000000001</v>
       </c>
       <c r="H31" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I31">
-        <v>0.115083</v>
+        <v>0.10815900000000001</v>
       </c>
       <c r="J31" t="s">
         <v>15</v>
@@ -10295,13 +10292,13 @@
         <v>16</v>
       </c>
       <c r="M31" s="4">
-        <v>3.1398469999999999E-5</v>
+        <v>5.0422459999999998E-5</v>
       </c>
       <c r="N31" t="s">
         <v>17</v>
       </c>
       <c r="O31">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T31" s="4"/>
     </row>
@@ -10313,25 +10310,25 @@
         <v>5</v>
       </c>
       <c r="C32">
-        <v>0.27616400000000002</v>
+        <v>0.28762399999999999</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
       <c r="E32">
-        <v>3.95328E-2</v>
+        <v>3.34741E-2</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32">
-        <v>0.195766</v>
+        <v>0.20896000000000001</v>
       </c>
       <c r="H32" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I32">
-        <v>0.115024</v>
+        <v>0.10813399999999999</v>
       </c>
       <c r="J32" t="s">
         <v>15</v>
@@ -10343,13 +10340,13 @@
         <v>16</v>
       </c>
       <c r="M32" s="4">
-        <v>3.0924959999999997E-5</v>
+        <v>5.0800190000000001E-5</v>
       </c>
       <c r="N32" t="s">
         <v>17</v>
       </c>
       <c r="O32">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T32" s="4"/>
     </row>
@@ -10361,25 +10358,25 @@
         <v>5</v>
       </c>
       <c r="C33">
-        <v>0.273393</v>
+        <v>0.26132300000000003</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
       </c>
       <c r="E33">
-        <v>3.9509099999999998E-2</v>
+        <v>3.3328299999999998E-2</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
       </c>
       <c r="G33">
-        <v>0.190022</v>
+        <v>0.18282000000000001</v>
       </c>
       <c r="H33" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I33">
-        <v>0.115004</v>
+        <v>0.10813300000000001</v>
       </c>
       <c r="J33" t="s">
         <v>15</v>
@@ -10391,13 +10388,13 @@
         <v>16</v>
       </c>
       <c r="M33" s="4">
-        <v>3.0513459999999999E-5</v>
+        <v>5.106113E-5</v>
       </c>
       <c r="N33" t="s">
         <v>17</v>
       </c>
       <c r="O33">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T33" s="4"/>
     </row>
@@ -10409,25 +10406,25 @@
         <v>5</v>
       </c>
       <c r="C34">
-        <v>0.28950199999999998</v>
+        <v>0.28195500000000001</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
       </c>
       <c r="E34">
-        <v>3.95152E-2</v>
+        <v>3.3417700000000002E-2</v>
       </c>
       <c r="F34" t="s">
         <v>13</v>
       </c>
       <c r="G34">
-        <v>0.20438200000000001</v>
+        <v>0.184616</v>
       </c>
       <c r="H34" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I34">
-        <v>0.115033</v>
+        <v>0.108125</v>
       </c>
       <c r="J34" t="s">
         <v>15</v>
@@ -10439,13 +10436,13 @@
         <v>16</v>
       </c>
       <c r="M34" s="4">
-        <v>3.0143600000000001E-5</v>
+        <v>5.137923E-5</v>
       </c>
       <c r="N34" t="s">
         <v>17</v>
       </c>
       <c r="O34">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T34" s="4"/>
     </row>
@@ -10457,25 +10454,25 @@
         <v>5</v>
       </c>
       <c r="C35">
-        <v>0.27557900000000002</v>
+        <v>0.25889000000000001</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
       </c>
       <c r="E35">
-        <v>3.9406099999999999E-2</v>
+        <v>3.33269E-2</v>
       </c>
       <c r="F35" t="s">
         <v>13</v>
       </c>
       <c r="G35">
-        <v>0.19239600000000001</v>
+        <v>0.184889</v>
       </c>
       <c r="H35" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I35">
-        <v>0.115036</v>
+        <v>0.108158</v>
       </c>
       <c r="J35" t="s">
         <v>15</v>
@@ -10487,13 +10484,13 @@
         <v>16</v>
       </c>
       <c r="M35" s="4">
-        <v>2.978132E-5</v>
+        <v>5.1819620000000002E-5</v>
       </c>
       <c r="N35" t="s">
         <v>17</v>
       </c>
       <c r="O35">
-        <v>6.6180000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T35" s="4"/>
     </row>
@@ -10505,43 +10502,43 @@
         <v>5</v>
       </c>
       <c r="C36">
-        <v>0.24607299999999999</v>
+        <v>0.274675</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
       </c>
       <c r="E36">
-        <v>3.9461700000000002E-2</v>
+        <v>3.3476800000000001E-2</v>
       </c>
       <c r="F36" t="s">
         <v>13</v>
       </c>
       <c r="G36">
-        <v>0.161939</v>
+        <v>0.19123499999999999</v>
       </c>
       <c r="H36" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I36">
-        <v>9.8611099999999993E-2</v>
+        <v>0.108168</v>
       </c>
       <c r="J36" t="s">
         <v>15</v>
       </c>
       <c r="K36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L36" t="s">
         <v>16</v>
       </c>
       <c r="M36" s="4">
-        <v>9.9946090000000001E-5</v>
+        <v>5.2521149999999998E-5</v>
       </c>
       <c r="N36" t="s">
         <v>17</v>
       </c>
       <c r="O36">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T36" s="4"/>
     </row>
@@ -10553,43 +10550,43 @@
         <v>5</v>
       </c>
       <c r="C37">
-        <v>0.252415</v>
+        <v>0.26636100000000001</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
       </c>
       <c r="E37">
-        <v>3.9509799999999998E-2</v>
+        <v>3.3355200000000002E-2</v>
       </c>
       <c r="F37" t="s">
         <v>13</v>
       </c>
       <c r="G37">
-        <v>0.16423299999999999</v>
+        <v>0.18803900000000001</v>
       </c>
       <c r="H37" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I37">
-        <v>9.85877E-2</v>
+        <v>0.108164</v>
       </c>
       <c r="J37" t="s">
         <v>15</v>
       </c>
       <c r="K37">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L37" t="s">
         <v>16</v>
       </c>
       <c r="M37" s="4">
-        <v>9.9038130000000005E-5</v>
+        <v>5.329E-5</v>
       </c>
       <c r="N37" t="s">
         <v>17</v>
       </c>
       <c r="O37">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T37" s="4"/>
     </row>
@@ -10601,43 +10598,43 @@
         <v>5</v>
       </c>
       <c r="C38">
-        <v>0.24890999999999999</v>
+        <v>0.26513799999999998</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
       </c>
       <c r="E38">
-        <v>3.95463E-2</v>
+        <v>3.3344400000000003E-2</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
       </c>
       <c r="G38">
-        <v>0.16047400000000001</v>
+        <v>0.18516299999999999</v>
       </c>
       <c r="H38" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I38">
-        <v>9.8627599999999996E-2</v>
+        <v>0.108139</v>
       </c>
       <c r="J38" t="s">
         <v>15</v>
       </c>
       <c r="K38">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L38" t="s">
         <v>16</v>
       </c>
       <c r="M38" s="4">
-        <v>9.8209690000000002E-5</v>
+        <v>5.3832290000000002E-5</v>
       </c>
       <c r="N38" t="s">
         <v>17</v>
       </c>
       <c r="O38">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T38" s="4"/>
     </row>
@@ -10649,43 +10646,43 @@
         <v>5</v>
       </c>
       <c r="C39">
-        <v>0.24371100000000001</v>
+        <v>0.27658500000000003</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
       </c>
       <c r="E39">
-        <v>3.9520600000000003E-2</v>
+        <v>3.3397799999999998E-2</v>
       </c>
       <c r="F39" t="s">
         <v>13</v>
       </c>
       <c r="G39">
-        <v>0.16317100000000001</v>
+        <v>0.196328</v>
       </c>
       <c r="H39" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I39">
-        <v>9.8592799999999994E-2</v>
+        <v>0.108149</v>
       </c>
       <c r="J39" t="s">
         <v>15</v>
       </c>
       <c r="K39">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L39" t="s">
         <v>16</v>
       </c>
       <c r="M39" s="4">
-        <v>9.7181210000000005E-5</v>
+        <v>5.3949439999999998E-5</v>
       </c>
       <c r="N39" t="s">
         <v>17</v>
       </c>
       <c r="O39">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T39" s="4"/>
     </row>
@@ -10697,43 +10694,43 @@
         <v>5</v>
       </c>
       <c r="C40">
-        <v>0.24268899999999999</v>
+        <v>0.27164100000000002</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
       </c>
       <c r="E40">
-        <v>3.9502700000000002E-2</v>
+        <v>3.3408199999999999E-2</v>
       </c>
       <c r="F40" t="s">
         <v>13</v>
       </c>
       <c r="G40">
-        <v>0.161995</v>
+        <v>0.19587299999999999</v>
       </c>
       <c r="H40" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I40">
-        <v>9.8564100000000002E-2</v>
+        <v>0.108155</v>
       </c>
       <c r="J40" t="s">
         <v>15</v>
       </c>
       <c r="K40">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L40" t="s">
         <v>16</v>
       </c>
       <c r="M40" s="4">
-        <v>9.6096480000000003E-5</v>
+        <v>5.3636730000000003E-5</v>
       </c>
       <c r="N40" t="s">
         <v>17</v>
       </c>
       <c r="O40">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T40" s="4"/>
     </row>
@@ -10745,43 +10742,43 @@
         <v>5</v>
       </c>
       <c r="C41">
-        <v>0.24451100000000001</v>
+        <v>0.27058599999999999</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
       </c>
       <c r="E41">
-        <v>3.9518900000000003E-2</v>
+        <v>3.3401699999999999E-2</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
       </c>
       <c r="G41">
-        <v>0.16109899999999999</v>
+        <v>0.190641</v>
       </c>
       <c r="H41" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I41">
-        <v>9.8628599999999997E-2</v>
+        <v>0.108138</v>
       </c>
       <c r="J41" t="s">
         <v>15</v>
       </c>
       <c r="K41">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L41" t="s">
         <v>16</v>
       </c>
       <c r="M41" s="4">
-        <v>9.4842450000000002E-5</v>
+        <v>5.2896119999999998E-5</v>
       </c>
       <c r="N41" t="s">
         <v>17</v>
       </c>
       <c r="O41">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T41" s="4"/>
     </row>
@@ -10793,43 +10790,43 @@
         <v>5</v>
       </c>
       <c r="C42">
-        <v>0.24605099999999999</v>
+        <v>0.26871600000000001</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
       <c r="E42">
-        <v>3.9451399999999998E-2</v>
+        <v>3.33788E-2</v>
       </c>
       <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42">
-        <v>0.16261200000000001</v>
+        <v>0.18382299999999999</v>
       </c>
       <c r="H42" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I42">
-        <v>9.8601999999999995E-2</v>
+        <v>0.108124</v>
       </c>
       <c r="J42" t="s">
         <v>15</v>
       </c>
       <c r="K42">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L42" t="s">
         <v>16</v>
       </c>
       <c r="M42" s="4">
-        <v>9.3462619999999997E-5</v>
+        <v>5.1805999999999998E-5</v>
       </c>
       <c r="N42" t="s">
         <v>17</v>
       </c>
       <c r="O42">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T42" s="4"/>
     </row>
@@ -10841,43 +10838,43 @@
         <v>5</v>
       </c>
       <c r="C43">
-        <v>0.24715000000000001</v>
+        <v>0.29079700000000003</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
       </c>
       <c r="E43">
-        <v>3.9520600000000003E-2</v>
+        <v>3.34956E-2</v>
       </c>
       <c r="F43" t="s">
         <v>13</v>
       </c>
       <c r="G43">
-        <v>0.16640199999999999</v>
+        <v>0.20896200000000001</v>
       </c>
       <c r="H43" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I43">
-        <v>9.87064E-2</v>
+        <v>0.10816199999999999</v>
       </c>
       <c r="J43" t="s">
         <v>15</v>
       </c>
       <c r="K43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L43" t="s">
         <v>16</v>
       </c>
       <c r="M43" s="4">
-        <v>9.1909679999999997E-5</v>
+        <v>5.0500390000000001E-5</v>
       </c>
       <c r="N43" t="s">
         <v>17</v>
       </c>
       <c r="O43">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T43" s="4"/>
     </row>
@@ -10889,43 +10886,43 @@
         <v>5</v>
       </c>
       <c r="C44">
-        <v>0.244537</v>
+        <v>0.26627099999999998</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
       </c>
       <c r="E44">
-        <v>3.9465199999999999E-2</v>
+        <v>3.3298500000000002E-2</v>
       </c>
       <c r="F44" t="s">
         <v>13</v>
       </c>
       <c r="G44">
-        <v>0.16401299999999999</v>
+        <v>0.18453900000000001</v>
       </c>
       <c r="H44" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I44">
-        <v>9.8577399999999996E-2</v>
+        <v>0.108164</v>
       </c>
       <c r="J44" t="s">
         <v>15</v>
       </c>
       <c r="K44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L44" t="s">
         <v>16</v>
       </c>
       <c r="M44" s="4">
-        <v>9.0158800000000002E-5</v>
+        <v>4.9082660000000001E-5</v>
       </c>
       <c r="N44" t="s">
         <v>17</v>
       </c>
       <c r="O44">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T44" s="4"/>
     </row>
@@ -10937,43 +10934,43 @@
         <v>5</v>
       </c>
       <c r="C45">
-        <v>0.25173899999999999</v>
+        <v>0.275503</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
       </c>
       <c r="E45">
-        <v>3.9522500000000002E-2</v>
+        <v>3.3486700000000001E-2</v>
       </c>
       <c r="F45" t="s">
         <v>13</v>
       </c>
       <c r="G45">
-        <v>0.16024099999999999</v>
+        <v>0.191714</v>
       </c>
       <c r="H45" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I45">
-        <v>9.8568199999999995E-2</v>
+        <v>0.108143</v>
       </c>
       <c r="J45" t="s">
         <v>15</v>
       </c>
       <c r="K45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L45" t="s">
         <v>16</v>
       </c>
       <c r="M45" s="4">
-        <v>8.8282439999999996E-5</v>
+        <v>4.7714930000000002E-5</v>
       </c>
       <c r="N45" t="s">
         <v>17</v>
       </c>
       <c r="O45">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T45" s="4"/>
     </row>
@@ -10985,43 +10982,43 @@
         <v>5</v>
       </c>
       <c r="C46">
-        <v>0.26013700000000001</v>
+        <v>0.27251999999999998</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
       </c>
       <c r="E46">
-        <v>3.9496400000000001E-2</v>
+        <v>3.3455100000000002E-2</v>
       </c>
       <c r="F46" t="s">
         <v>13</v>
       </c>
       <c r="G46">
-        <v>0.172234</v>
+        <v>0.197464</v>
       </c>
       <c r="H46" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I46">
-        <v>9.8613199999999998E-2</v>
+        <v>0.10814799999999999</v>
       </c>
       <c r="J46" t="s">
         <v>15</v>
       </c>
       <c r="K46">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L46" t="s">
         <v>16</v>
       </c>
       <c r="M46" s="4">
-        <v>8.6303239999999993E-5</v>
+        <v>4.6460069999999997E-5</v>
       </c>
       <c r="N46" t="s">
         <v>17</v>
       </c>
       <c r="O46">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T46" s="4"/>
     </row>
@@ -11033,43 +11030,43 @@
         <v>5</v>
       </c>
       <c r="C47">
-        <v>0.24542600000000001</v>
+        <v>0.270617</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
       </c>
       <c r="E47">
-        <v>3.9575699999999998E-2</v>
+        <v>3.3378499999999998E-2</v>
       </c>
       <c r="F47" t="s">
         <v>13</v>
       </c>
       <c r="G47">
-        <v>0.162495</v>
+        <v>0.19278999999999999</v>
       </c>
       <c r="H47" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I47">
-        <v>9.8598900000000003E-2</v>
+        <v>0.108158</v>
       </c>
       <c r="J47" t="s">
         <v>15</v>
       </c>
       <c r="K47">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L47" t="s">
         <v>16</v>
       </c>
       <c r="M47" s="4">
-        <v>8.425753E-5</v>
+        <v>4.5393930000000001E-5</v>
       </c>
       <c r="N47" t="s">
         <v>17</v>
       </c>
       <c r="O47">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T47" s="4"/>
     </row>
@@ -11081,43 +11078,43 @@
         <v>5</v>
       </c>
       <c r="C48">
-        <v>0.26201799999999997</v>
+        <v>0.27374599999999999</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
       </c>
       <c r="E48">
-        <v>3.9478899999999997E-2</v>
+        <v>3.3433999999999998E-2</v>
       </c>
       <c r="F48" t="s">
         <v>13</v>
       </c>
       <c r="G48">
-        <v>0.16578399999999999</v>
+        <v>0.197328</v>
       </c>
       <c r="H48" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I48">
-        <v>9.8629599999999998E-2</v>
+        <v>0.10813399999999999</v>
       </c>
       <c r="J48" t="s">
         <v>15</v>
       </c>
       <c r="K48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L48" t="s">
         <v>16</v>
       </c>
       <c r="M48" s="4">
-        <v>8.2176370000000006E-5</v>
+        <v>4.445064E-5</v>
       </c>
       <c r="N48" t="s">
         <v>17</v>
       </c>
       <c r="O48">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T48" s="4"/>
     </row>
@@ -11129,43 +11126,43 @@
         <v>5</v>
       </c>
       <c r="C49">
-        <v>0.24087800000000001</v>
+        <v>0.28045900000000001</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
       </c>
       <c r="E49">
-        <v>3.94597E-2</v>
+        <v>3.34227E-2</v>
       </c>
       <c r="F49" t="s">
         <v>13</v>
       </c>
       <c r="G49">
-        <v>0.160465</v>
+        <v>0.198356</v>
       </c>
       <c r="H49" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I49">
-        <v>9.8636799999999997E-2</v>
+        <v>0.10816099999999999</v>
       </c>
       <c r="J49" t="s">
         <v>15</v>
       </c>
       <c r="K49">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L49" t="s">
         <v>16</v>
       </c>
       <c r="M49" s="4">
-        <v>8.0115859999999994E-5</v>
+        <v>4.3599320000000003E-5</v>
       </c>
       <c r="N49" t="s">
         <v>17</v>
       </c>
       <c r="O49">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T49" s="4"/>
     </row>
@@ -11177,43 +11174,43 @@
         <v>5</v>
       </c>
       <c r="C50">
-        <v>0.25711000000000001</v>
+        <v>0.27660200000000001</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50">
-        <v>3.95526E-2</v>
+        <v>3.3305300000000003E-2</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>
       </c>
       <c r="G50">
-        <v>0.17645</v>
+        <v>0.19758800000000001</v>
       </c>
       <c r="H50" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I50">
-        <v>9.8602999999999996E-2</v>
+        <v>0.108117</v>
       </c>
       <c r="J50" t="s">
         <v>15</v>
       </c>
       <c r="K50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L50" t="s">
         <v>16</v>
       </c>
       <c r="M50" s="4">
-        <v>7.8031149999999996E-5</v>
+        <v>4.2745679999999998E-5</v>
       </c>
       <c r="N50" t="s">
         <v>17</v>
       </c>
       <c r="O50">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T50" s="4"/>
     </row>
@@ -11225,43 +11222,43 @@
         <v>5</v>
       </c>
       <c r="C51">
-        <v>0.25220799999999999</v>
+        <v>0.262685</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51">
-        <v>3.9582800000000001E-2</v>
+        <v>3.3565600000000001E-2</v>
       </c>
       <c r="F51" t="s">
         <v>13</v>
       </c>
       <c r="G51">
-        <v>0.16580300000000001</v>
+        <v>0.185866</v>
       </c>
       <c r="H51" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I51">
-        <v>9.8600900000000005E-2</v>
+        <v>0.10824499999999999</v>
       </c>
       <c r="J51" t="s">
         <v>15</v>
       </c>
       <c r="K51">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L51" t="s">
         <v>16</v>
       </c>
       <c r="M51" s="4">
-        <v>7.5949679999999994E-5</v>
+        <v>4.1884439999999998E-5</v>
       </c>
       <c r="N51" t="s">
         <v>17</v>
       </c>
       <c r="O51">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T51" s="4"/>
     </row>
@@ -11273,43 +11270,43 @@
         <v>5</v>
       </c>
       <c r="C52">
-        <v>0.24596399999999999</v>
+        <v>0.27452500000000002</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52">
-        <v>3.9552799999999999E-2</v>
+        <v>3.34051E-2</v>
       </c>
       <c r="F52" t="s">
         <v>13</v>
       </c>
       <c r="G52">
-        <v>0.161994</v>
+        <v>0.19545799999999999</v>
       </c>
       <c r="H52" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I52">
-        <v>9.8633799999999994E-2</v>
+        <v>0.108155</v>
       </c>
       <c r="J52" t="s">
         <v>15</v>
       </c>
       <c r="K52">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L52" t="s">
         <v>16</v>
       </c>
       <c r="M52" s="4">
-        <v>7.3860390000000001E-5</v>
+        <v>4.099234E-5</v>
       </c>
       <c r="N52" t="s">
         <v>17</v>
       </c>
       <c r="O52">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T52" s="4"/>
     </row>
@@ -11321,43 +11318,43 @@
         <v>5</v>
       </c>
       <c r="C53">
-        <v>0.25285299999999999</v>
+        <v>0.28123799999999999</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
       </c>
       <c r="E53">
-        <v>3.9481200000000001E-2</v>
+        <v>3.3300200000000002E-2</v>
       </c>
       <c r="F53" t="s">
         <v>13</v>
       </c>
       <c r="G53">
-        <v>0.165406</v>
+        <v>0.19983999999999999</v>
       </c>
       <c r="H53" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I53">
-        <v>9.8634700000000006E-2</v>
+        <v>0.10816000000000001</v>
       </c>
       <c r="J53" t="s">
         <v>15</v>
       </c>
       <c r="K53">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L53" t="s">
         <v>16</v>
       </c>
       <c r="M53" s="4">
-        <v>7.1803119999999998E-5</v>
+        <v>4.0073819999999997E-5</v>
       </c>
       <c r="N53" t="s">
         <v>17</v>
       </c>
       <c r="O53">
-        <v>6.5170000000000003</v>
+        <v>6.9829999999999997</v>
       </c>
       <c r="T53" s="4"/>
     </row>
@@ -11368,37 +11365,37 @@
       <c r="B55" s="5"/>
       <c r="C55" s="6">
         <f>AVERAGE(C3:C53)</f>
-        <v>0.25569339411764708</v>
+        <v>0.26070811960784313</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6">
         <f>AVERAGE(E3:E53)</f>
-        <v>3.724837215686274E-2</v>
+        <v>3.1479316549019601E-2</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6">
         <f>AVERAGE(G3:G53)</f>
-        <v>0.17531840901960788</v>
+        <v>0.18451706156862752</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="6">
         <f>AVERAGE(I3:I53)</f>
-        <v>0.10473648666666664</v>
+        <v>0.1042005780392157</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6">
         <f>AVERAGE(K3:K53)</f>
-        <v>6.7647058823529411</v>
+        <v>7.1568627450980395</v>
       </c>
       <c r="L55" s="6"/>
       <c r="M55" s="6">
         <f>AVERAGE(M3:M53)</f>
-        <v>6.2146204901960793E-5</v>
+        <v>5.2378614509803935E-5</v>
       </c>
       <c r="N55" s="6"/>
       <c r="O55" s="6">
         <f>AVERAGE(O3:O53)</f>
-        <v>6.2479411764705857</v>
+        <v>6.6505882352941201</v>
       </c>
       <c r="P55" s="6"/>
       <c r="Q55" s="6"/>
@@ -11582,8 +11579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01678F02-6852-1843-B1D7-578F6A92EC72}">
   <dimension ref="A1:U155"/>
   <sheetViews>
-    <sheetView zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="O53" sqref="O3:O53"/>
+    <sheetView topLeftCell="F38" zoomScale="113" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11645,25 +11642,25 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>2.6627999999999999E-2</v>
+        <v>4.2704899999999997E-2</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3">
-        <v>5.2366399999999999E-3</v>
+        <v>4.87894E-3</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
       </c>
       <c r="G3">
-        <v>1.21353E-2</v>
+        <v>1.35342E-2</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
       </c>
       <c r="I3">
-        <v>8.8852500000000008E-3</v>
+        <v>8.3374699999999996E-3</v>
       </c>
       <c r="J3" t="s">
         <v>15</v>
@@ -11681,7 +11678,7 @@
         <v>17</v>
       </c>
       <c r="O3">
-        <v>0.72899999999999998</v>
+        <v>1.0940000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="20" customHeight="1">
@@ -11689,25 +11686,25 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2.8677299999999999E-2</v>
+        <v>3.1021900000000002E-2</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4">
-        <v>5.2445800000000004E-3</v>
+        <v>4.8718099999999999E-3</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4">
-        <v>1.41058E-2</v>
+        <v>1.379E-2</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
       </c>
       <c r="I4">
-        <v>8.8617000000000001E-3</v>
+        <v>8.2728000000000003E-3</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
@@ -11725,7 +11722,7 @@
         <v>17</v>
       </c>
       <c r="O4">
-        <v>0.72899999999999998</v>
+        <v>1.0940000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="20" customHeight="1">
@@ -11733,25 +11730,25 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>4.2565600000000002E-2</v>
+        <v>3.07377E-2</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5">
-        <v>5.22406E-3</v>
+        <v>4.8758100000000004E-3</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="G5">
-        <v>1.28215E-2</v>
+        <v>1.13575E-2</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="I5">
-        <v>8.9190399999999996E-3</v>
+        <v>8.2974699999999995E-3</v>
       </c>
       <c r="J5" t="s">
         <v>15</v>
@@ -11769,7 +11766,7 @@
         <v>17</v>
       </c>
       <c r="O5">
-        <v>0.72899999999999998</v>
+        <v>1.0940000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="20" customHeight="1">
@@ -11777,25 +11774,25 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0.57511800000000002</v>
+        <v>0.567411</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6">
-        <v>0.212058</v>
+        <v>0.21193100000000001</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6">
-        <v>0.22592899999999999</v>
+        <v>0.22783400000000001</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
       <c r="I6">
-        <v>0.162157</v>
+        <v>0.16223000000000001</v>
       </c>
       <c r="J6" t="s">
         <v>15</v>
@@ -11813,7 +11810,7 @@
         <v>17</v>
       </c>
       <c r="O6">
-        <v>10.054</v>
+        <v>10.419</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="20" customHeight="1">
@@ -11821,25 +11818,25 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.52259</v>
+        <v>0.53141000000000005</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7">
-        <v>0.212147</v>
+        <v>0.21227499999999999</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
       <c r="G7">
-        <v>0.19017500000000001</v>
+        <v>0.192907</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
       </c>
       <c r="I7">
-        <v>0.13513700000000001</v>
+        <v>0.13522600000000001</v>
       </c>
       <c r="J7" t="s">
         <v>15</v>
@@ -11857,7 +11854,7 @@
         <v>17</v>
       </c>
       <c r="O7">
-        <v>9.952</v>
+        <v>10.317</v>
       </c>
       <c r="S7" s="4"/>
     </row>
@@ -11866,25 +11863,25 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>0.53453899999999999</v>
+        <v>0.53842299999999998</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8">
-        <v>0.21184800000000001</v>
+        <v>0.211896</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8">
-        <v>0.186999</v>
+        <v>0.19126299999999999</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
       <c r="I8">
-        <v>0.135103</v>
+        <v>0.13514899999999999</v>
       </c>
       <c r="J8" t="s">
         <v>15</v>
@@ -11902,7 +11899,7 @@
         <v>17</v>
       </c>
       <c r="O8">
-        <v>9.952</v>
+        <v>10.317</v>
       </c>
       <c r="S8" s="4"/>
     </row>
@@ -11911,25 +11908,25 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>0.53261199999999997</v>
+        <v>0.53577300000000005</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
       <c r="E9">
-        <v>0.21218899999999999</v>
+        <v>0.21238099999999999</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
       <c r="G9">
-        <v>0.194466</v>
+        <v>0.19288</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
       </c>
       <c r="I9">
-        <v>0.13505600000000001</v>
+        <v>0.135161</v>
       </c>
       <c r="J9" t="s">
         <v>15</v>
@@ -11947,7 +11944,7 @@
         <v>17</v>
       </c>
       <c r="O9">
-        <v>9.952</v>
+        <v>10.317</v>
       </c>
       <c r="S9" s="4"/>
     </row>
@@ -11956,25 +11953,25 @@
         <v>5</v>
       </c>
       <c r="C10">
-        <v>0.52848399999999995</v>
+        <v>0.55539899999999998</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10">
-        <v>0.21216399999999999</v>
+        <v>0.21193999999999999</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
       <c r="G10">
-        <v>0.191109</v>
+        <v>0.193191</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
       </c>
       <c r="I10">
-        <v>0.13520399999999999</v>
+        <v>0.13515199999999999</v>
       </c>
       <c r="J10" t="s">
         <v>15</v>
@@ -11992,7 +11989,7 @@
         <v>17</v>
       </c>
       <c r="O10">
-        <v>9.952</v>
+        <v>10.317</v>
       </c>
       <c r="S10" s="4"/>
     </row>
@@ -12001,25 +11998,25 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>0.52360799999999996</v>
+        <v>0.54637000000000002</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11">
-        <v>0.212087</v>
+        <v>0.21195</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11">
-        <v>0.19025600000000001</v>
+        <v>0.19040199999999999</v>
       </c>
       <c r="H11" t="s">
         <v>14</v>
       </c>
       <c r="I11">
-        <v>0.135079</v>
+        <v>0.135133</v>
       </c>
       <c r="J11" t="s">
         <v>15</v>
@@ -12037,7 +12034,7 @@
         <v>17</v>
       </c>
       <c r="O11">
-        <v>9.952</v>
+        <v>10.317</v>
       </c>
       <c r="S11" s="4"/>
     </row>
@@ -12046,25 +12043,25 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>0.52264999999999995</v>
+        <v>0.53188100000000005</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12">
-        <v>0.21210899999999999</v>
+        <v>0.21220900000000001</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
       <c r="G12">
-        <v>0.18695500000000001</v>
+        <v>0.188439</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
       </c>
       <c r="I12">
-        <v>0.13515199999999999</v>
+        <v>0.13511999999999999</v>
       </c>
       <c r="J12" t="s">
         <v>15</v>
@@ -12082,7 +12079,7 @@
         <v>17</v>
       </c>
       <c r="O12">
-        <v>9.952</v>
+        <v>10.317</v>
       </c>
       <c r="S12" s="4"/>
     </row>
@@ -12091,25 +12088,25 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <v>0.52737299999999998</v>
+        <v>0.52805899999999995</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13">
-        <v>0.21181</v>
+        <v>0.21199100000000001</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13">
-        <v>0.18856300000000001</v>
+        <v>0.19006500000000001</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
       </c>
       <c r="I13">
-        <v>0.13506199999999999</v>
+        <v>0.13513</v>
       </c>
       <c r="J13" t="s">
         <v>15</v>
@@ -12127,7 +12124,7 @@
         <v>17</v>
       </c>
       <c r="O13">
-        <v>9.952</v>
+        <v>10.317</v>
       </c>
       <c r="S13" s="4"/>
     </row>
@@ -12136,25 +12133,25 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>0.53649999999999998</v>
+        <v>0.54805300000000001</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14">
-        <v>0.211976</v>
+        <v>0.21232699999999999</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
       </c>
       <c r="G14">
-        <v>0.19420999999999999</v>
+        <v>0.19586100000000001</v>
       </c>
       <c r="H14" t="s">
         <v>14</v>
       </c>
       <c r="I14">
-        <v>0.13511600000000001</v>
+        <v>0.13515199999999999</v>
       </c>
       <c r="J14" t="s">
         <v>15</v>
@@ -12172,7 +12169,7 @@
         <v>17</v>
       </c>
       <c r="O14">
-        <v>9.952</v>
+        <v>10.317</v>
       </c>
       <c r="S14" s="4"/>
     </row>
@@ -12181,7 +12178,7 @@
         <v>5</v>
       </c>
       <c r="C15">
-        <v>0.53008</v>
+        <v>0.53506900000000002</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -12193,13 +12190,13 @@
         <v>13</v>
       </c>
       <c r="G15">
-        <v>0.18847</v>
+        <v>0.19517399999999999</v>
       </c>
       <c r="H15" t="s">
         <v>14</v>
       </c>
       <c r="I15">
-        <v>0.135042</v>
+        <v>0.13516700000000001</v>
       </c>
       <c r="J15" t="s">
         <v>15</v>
@@ -12217,7 +12214,7 @@
         <v>17</v>
       </c>
       <c r="O15">
-        <v>9.952</v>
+        <v>10.317</v>
       </c>
       <c r="S15" s="4"/>
     </row>
@@ -12226,25 +12223,25 @@
         <v>5</v>
       </c>
       <c r="C16">
-        <v>0.56327099999999997</v>
+        <v>0.57111100000000004</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16">
-        <v>0.21191399999999999</v>
+        <v>0.212005</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
       </c>
       <c r="G16">
-        <v>0.22873399999999999</v>
+        <v>0.23433100000000001</v>
       </c>
       <c r="H16" t="s">
         <v>14</v>
       </c>
       <c r="I16">
-        <v>0.162157</v>
+        <v>0.16217300000000001</v>
       </c>
       <c r="J16" t="s">
         <v>15</v>
@@ -12262,7 +12259,7 @@
         <v>17</v>
       </c>
       <c r="O16">
-        <v>10.054</v>
+        <v>10.419</v>
       </c>
       <c r="S16" s="4"/>
     </row>
@@ -12271,25 +12268,25 @@
         <v>5</v>
       </c>
       <c r="C17">
-        <v>0.55759099999999995</v>
+        <v>0.56835100000000005</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17">
-        <v>0.21229700000000001</v>
+        <v>0.21194099999999999</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
       <c r="G17">
-        <v>0.22448199999999999</v>
+        <v>0.23505000000000001</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
       </c>
       <c r="I17">
-        <v>0.16219800000000001</v>
+        <v>0.16225700000000001</v>
       </c>
       <c r="J17" t="s">
         <v>15</v>
@@ -12307,7 +12304,7 @@
         <v>17</v>
       </c>
       <c r="O17">
-        <v>10.054</v>
+        <v>10.419</v>
       </c>
       <c r="S17" s="4"/>
     </row>
@@ -12316,25 +12313,25 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>0.56577200000000005</v>
+        <v>0.56057400000000002</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18">
-        <v>0.21211199999999999</v>
+        <v>0.211926</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
       </c>
       <c r="G18">
-        <v>0.22819600000000001</v>
+        <v>0.226325</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
       </c>
       <c r="I18">
-        <v>0.16208400000000001</v>
+        <v>0.162214</v>
       </c>
       <c r="J18" t="s">
         <v>15</v>
@@ -12352,7 +12349,7 @@
         <v>17</v>
       </c>
       <c r="O18">
-        <v>10.054</v>
+        <v>10.419</v>
       </c>
       <c r="S18" s="4"/>
     </row>
@@ -12361,25 +12358,25 @@
         <v>5</v>
       </c>
       <c r="C19">
-        <v>0.56413599999999997</v>
+        <v>0.57582199999999994</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19">
-        <v>0.21204700000000001</v>
+        <v>0.21240999999999999</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
       <c r="G19">
-        <v>0.229795</v>
+        <v>0.23488200000000001</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
       </c>
       <c r="I19">
-        <v>0.16214200000000001</v>
+        <v>0.16218099999999999</v>
       </c>
       <c r="J19" t="s">
         <v>15</v>
@@ -12397,7 +12394,7 @@
         <v>17</v>
       </c>
       <c r="O19">
-        <v>10.054</v>
+        <v>10.419</v>
       </c>
       <c r="S19" s="4"/>
     </row>
@@ -12406,25 +12403,25 @@
         <v>5</v>
       </c>
       <c r="C20">
-        <v>0.57110099999999997</v>
+        <v>0.57827200000000001</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
       <c r="E20">
-        <v>0.21185999999999999</v>
+        <v>0.212286</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
       <c r="G20">
-        <v>0.22983899999999999</v>
+        <v>0.23739199999999999</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
       </c>
       <c r="I20">
-        <v>0.162075</v>
+        <v>0.16222500000000001</v>
       </c>
       <c r="J20" t="s">
         <v>15</v>
@@ -12442,7 +12439,7 @@
         <v>17</v>
       </c>
       <c r="O20">
-        <v>10.054</v>
+        <v>10.419</v>
       </c>
       <c r="S20" s="4"/>
     </row>
@@ -12451,25 +12448,25 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <v>0.56820800000000005</v>
+        <v>0.57602200000000003</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
       </c>
       <c r="E21">
-        <v>0.21233399999999999</v>
+        <v>0.211872</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21">
-        <v>0.22966</v>
+        <v>0.23360600000000001</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
       </c>
       <c r="I21">
-        <v>0.162138</v>
+        <v>0.162271</v>
       </c>
       <c r="J21" t="s">
         <v>15</v>
@@ -12487,7 +12484,7 @@
         <v>17</v>
       </c>
       <c r="O21">
-        <v>10.054</v>
+        <v>10.419</v>
       </c>
       <c r="S21" s="4"/>
     </row>
@@ -12496,25 +12493,25 @@
         <v>5</v>
       </c>
       <c r="C22">
-        <v>0.57177199999999995</v>
+        <v>0.59100900000000001</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
       <c r="E22">
-        <v>0.21218999999999999</v>
+        <v>0.212171</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22">
-        <v>0.23480300000000001</v>
+        <v>0.242872</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
       </c>
       <c r="I22">
-        <v>0.16207299999999999</v>
+        <v>0.16222800000000001</v>
       </c>
       <c r="J22" t="s">
         <v>15</v>
@@ -12532,7 +12529,7 @@
         <v>17</v>
       </c>
       <c r="O22">
-        <v>10.054</v>
+        <v>10.419</v>
       </c>
       <c r="S22" s="4"/>
     </row>
@@ -12541,25 +12538,25 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <v>0.56314299999999995</v>
+        <v>0.57896099999999995</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23">
-        <v>0.212037</v>
+        <v>0.21202499999999999</v>
       </c>
       <c r="F23" t="s">
         <v>13</v>
       </c>
       <c r="G23">
-        <v>0.22874700000000001</v>
+        <v>0.23306299999999999</v>
       </c>
       <c r="H23" t="s">
         <v>14</v>
       </c>
       <c r="I23">
-        <v>0.162249</v>
+        <v>0.16224</v>
       </c>
       <c r="J23" t="s">
         <v>15</v>
@@ -12577,7 +12574,7 @@
         <v>17</v>
       </c>
       <c r="O23">
-        <v>10.054</v>
+        <v>10.451000000000001</v>
       </c>
       <c r="S23" s="4"/>
     </row>
@@ -12586,25 +12583,25 @@
         <v>5</v>
       </c>
       <c r="C24">
-        <v>0.55882299999999996</v>
+        <v>0.57086000000000003</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
       <c r="E24">
-        <v>0.211955</v>
+        <v>0.21237500000000001</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
       </c>
       <c r="G24">
-        <v>0.226191</v>
+        <v>0.23610700000000001</v>
       </c>
       <c r="H24" t="s">
         <v>14</v>
       </c>
       <c r="I24">
-        <v>0.162189</v>
+        <v>0.16222400000000001</v>
       </c>
       <c r="J24" t="s">
         <v>15</v>
@@ -12622,7 +12619,7 @@
         <v>17</v>
       </c>
       <c r="O24">
-        <v>10.054</v>
+        <v>10.458</v>
       </c>
       <c r="S24" s="4"/>
     </row>
@@ -12631,25 +12628,25 @@
         <v>5</v>
       </c>
       <c r="C25">
-        <v>0.58055500000000004</v>
+        <v>0.580816</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
       <c r="E25">
-        <v>0.21206700000000001</v>
+        <v>0.21216399999999999</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25">
-        <v>0.22903899999999999</v>
+        <v>0.237263</v>
       </c>
       <c r="H25" t="s">
         <v>14</v>
       </c>
       <c r="I25">
-        <v>0.162247</v>
+        <v>0.16212799999999999</v>
       </c>
       <c r="J25" t="s">
         <v>15</v>
@@ -12667,7 +12664,7 @@
         <v>17</v>
       </c>
       <c r="O25">
-        <v>10.054</v>
+        <v>10.458</v>
       </c>
       <c r="S25" s="4"/>
     </row>
@@ -12676,25 +12673,25 @@
         <v>5</v>
       </c>
       <c r="C26">
-        <v>0.56006999999999996</v>
+        <v>0.56252000000000002</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
       <c r="E26">
-        <v>0.212033</v>
+        <v>0.21216199999999999</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
       </c>
       <c r="G26">
-        <v>0.22767200000000001</v>
+        <v>0.225799</v>
       </c>
       <c r="H26" t="s">
         <v>14</v>
       </c>
       <c r="I26">
-        <v>0.16214000000000001</v>
+        <v>0.162194</v>
       </c>
       <c r="J26" t="s">
         <v>15</v>
@@ -12712,7 +12709,7 @@
         <v>17</v>
       </c>
       <c r="O26">
-        <v>10.054</v>
+        <v>10.458</v>
       </c>
       <c r="S26" s="4"/>
     </row>
@@ -12721,25 +12718,25 @@
         <v>5</v>
       </c>
       <c r="C27">
-        <v>0.55792600000000003</v>
+        <v>0.57555999999999996</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
       </c>
       <c r="E27">
-        <v>0.21198800000000001</v>
+        <v>0.21187800000000001</v>
       </c>
       <c r="F27" t="s">
         <v>13</v>
       </c>
       <c r="G27">
-        <v>0.22534399999999999</v>
+        <v>0.229515</v>
       </c>
       <c r="H27" t="s">
         <v>14</v>
       </c>
       <c r="I27">
-        <v>0.16223799999999999</v>
+        <v>0.162135</v>
       </c>
       <c r="J27" t="s">
         <v>15</v>
@@ -12757,7 +12754,7 @@
         <v>17</v>
       </c>
       <c r="O27">
-        <v>10.054</v>
+        <v>10.458</v>
       </c>
       <c r="S27" s="4"/>
     </row>
@@ -12766,25 +12763,25 @@
         <v>5</v>
       </c>
       <c r="C28">
-        <v>0.57397900000000002</v>
+        <v>0.57194900000000004</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
       </c>
       <c r="E28">
-        <v>0.212341</v>
+        <v>0.21213699999999999</v>
       </c>
       <c r="F28" t="s">
         <v>13</v>
       </c>
       <c r="G28">
-        <v>0.228573</v>
+        <v>0.22761400000000001</v>
       </c>
       <c r="H28" t="s">
         <v>14</v>
       </c>
       <c r="I28">
-        <v>0.16216</v>
+        <v>0.162077</v>
       </c>
       <c r="J28" t="s">
         <v>15</v>
@@ -12802,7 +12799,7 @@
         <v>17</v>
       </c>
       <c r="O28">
-        <v>10.054</v>
+        <v>10.458</v>
       </c>
       <c r="S28" s="4"/>
     </row>
@@ -12811,25 +12808,25 @@
         <v>5</v>
       </c>
       <c r="C29">
-        <v>0.57128599999999996</v>
+        <v>0.57743900000000004</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
       <c r="E29">
-        <v>0.21174100000000001</v>
+        <v>0.21213399999999999</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
       </c>
       <c r="G29">
-        <v>0.229988</v>
+        <v>0.23977599999999999</v>
       </c>
       <c r="H29" t="s">
         <v>14</v>
       </c>
       <c r="I29">
-        <v>0.162105</v>
+        <v>0.162159</v>
       </c>
       <c r="J29" t="s">
         <v>15</v>
@@ -12847,7 +12844,7 @@
         <v>17</v>
       </c>
       <c r="O29">
-        <v>10.054</v>
+        <v>10.458</v>
       </c>
       <c r="S29" s="4"/>
     </row>
@@ -12856,25 +12853,25 @@
         <v>5</v>
       </c>
       <c r="C30">
-        <v>0.60334399999999999</v>
+        <v>0.61629500000000004</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
       </c>
       <c r="E30">
-        <v>0.212174</v>
+        <v>0.21162500000000001</v>
       </c>
       <c r="F30" t="s">
         <v>13</v>
       </c>
       <c r="G30">
-        <v>0.26461499999999999</v>
+        <v>0.28029599999999999</v>
       </c>
       <c r="H30" t="s">
         <v>14</v>
       </c>
       <c r="I30">
-        <v>0.189244</v>
+        <v>0.18921299999999999</v>
       </c>
       <c r="J30" t="s">
         <v>15</v>
@@ -12892,7 +12889,7 @@
         <v>17</v>
       </c>
       <c r="O30">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S30" s="4"/>
     </row>
@@ -12901,25 +12898,25 @@
         <v>5</v>
       </c>
       <c r="C31">
-        <v>0.607657</v>
+        <v>0.611487</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31">
-        <v>0.21210200000000001</v>
+        <v>0.21193600000000001</v>
       </c>
       <c r="F31" t="s">
         <v>13</v>
       </c>
       <c r="G31">
-        <v>0.26452199999999998</v>
+        <v>0.26778800000000003</v>
       </c>
       <c r="H31" t="s">
         <v>14</v>
       </c>
       <c r="I31">
-        <v>0.18909599999999999</v>
+        <v>0.18906700000000001</v>
       </c>
       <c r="J31" t="s">
         <v>15</v>
@@ -12937,7 +12934,7 @@
         <v>17</v>
       </c>
       <c r="O31">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S31" s="4"/>
     </row>
@@ -12946,25 +12943,25 @@
         <v>5</v>
       </c>
       <c r="C32">
-        <v>0.59881899999999999</v>
+        <v>0.63051000000000001</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
       </c>
       <c r="E32">
-        <v>0.212146</v>
+        <v>0.212147</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32">
-        <v>0.26263599999999998</v>
+        <v>0.28827999999999998</v>
       </c>
       <c r="H32" t="s">
         <v>14</v>
       </c>
       <c r="I32">
-        <v>0.18917900000000001</v>
+        <v>0.189113</v>
       </c>
       <c r="J32" t="s">
         <v>15</v>
@@ -12982,7 +12979,7 @@
         <v>17</v>
       </c>
       <c r="O32">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S32" s="4"/>
     </row>
@@ -12991,25 +12988,25 @@
         <v>5</v>
       </c>
       <c r="C33">
-        <v>0.59716100000000005</v>
+        <v>0.608927</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
       </c>
       <c r="E33">
-        <v>0.21218000000000001</v>
+        <v>0.21158399999999999</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
       </c>
       <c r="G33">
-        <v>0.26367699999999999</v>
+        <v>0.27654299999999998</v>
       </c>
       <c r="H33" t="s">
         <v>14</v>
       </c>
       <c r="I33">
-        <v>0.18923000000000001</v>
+        <v>0.18914700000000001</v>
       </c>
       <c r="J33" t="s">
         <v>15</v>
@@ -13027,7 +13024,7 @@
         <v>17</v>
       </c>
       <c r="O33">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S33" s="4"/>
     </row>
@@ -13036,25 +13033,25 @@
         <v>5</v>
       </c>
       <c r="C34">
-        <v>0.59987599999999996</v>
+        <v>0.63607199999999997</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
       </c>
       <c r="E34">
-        <v>0.21224499999999999</v>
+        <v>0.21224199999999999</v>
       </c>
       <c r="F34" t="s">
         <v>13</v>
       </c>
       <c r="G34">
-        <v>0.26522699999999999</v>
+        <v>0.29033599999999998</v>
       </c>
       <c r="H34" t="s">
         <v>14</v>
       </c>
       <c r="I34">
-        <v>0.18918399999999999</v>
+        <v>0.18914700000000001</v>
       </c>
       <c r="J34" t="s">
         <v>15</v>
@@ -13072,7 +13069,7 @@
         <v>17</v>
       </c>
       <c r="O34">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S34" s="4"/>
     </row>
@@ -13081,25 +13078,25 @@
         <v>5</v>
       </c>
       <c r="C35">
-        <v>0.60633599999999999</v>
+        <v>0.60861299999999996</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
       </c>
       <c r="E35">
-        <v>0.21213899999999999</v>
+        <v>0.21196300000000001</v>
       </c>
       <c r="F35" t="s">
         <v>13</v>
       </c>
       <c r="G35">
-        <v>0.26533000000000001</v>
+        <v>0.27002100000000001</v>
       </c>
       <c r="H35" t="s">
         <v>14</v>
       </c>
       <c r="I35">
-        <v>0.189192</v>
+        <v>0.18920100000000001</v>
       </c>
       <c r="J35" t="s">
         <v>15</v>
@@ -13117,7 +13114,7 @@
         <v>17</v>
       </c>
       <c r="O35">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S35" s="4"/>
     </row>
@@ -13126,25 +13123,25 @@
         <v>5</v>
       </c>
       <c r="C36">
-        <v>0.60599199999999998</v>
+        <v>0.62420100000000001</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
       </c>
       <c r="E36">
-        <v>0.21190999999999999</v>
+        <v>0.21182899999999999</v>
       </c>
       <c r="F36" t="s">
         <v>13</v>
       </c>
       <c r="G36">
-        <v>0.26184499999999999</v>
+        <v>0.27262999999999998</v>
       </c>
       <c r="H36" t="s">
         <v>14</v>
       </c>
       <c r="I36">
-        <v>0.189196</v>
+        <v>0.18915100000000001</v>
       </c>
       <c r="J36" t="s">
         <v>15</v>
@@ -13162,7 +13159,7 @@
         <v>17</v>
       </c>
       <c r="O36">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S36" s="4"/>
     </row>
@@ -13171,25 +13168,25 @@
         <v>5</v>
       </c>
       <c r="C37">
-        <v>0.60262300000000002</v>
+        <v>0.60583600000000004</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
       </c>
       <c r="E37">
-        <v>0.21206700000000001</v>
+        <v>0.21201600000000001</v>
       </c>
       <c r="F37" t="s">
         <v>13</v>
       </c>
       <c r="G37">
-        <v>0.26462999999999998</v>
+        <v>0.26734999999999998</v>
       </c>
       <c r="H37" t="s">
         <v>14</v>
       </c>
       <c r="I37">
-        <v>0.189165</v>
+        <v>0.18920100000000001</v>
       </c>
       <c r="J37" t="s">
         <v>15</v>
@@ -13207,7 +13204,7 @@
         <v>17</v>
       </c>
       <c r="O37">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S37" s="4"/>
     </row>
@@ -13216,25 +13213,25 @@
         <v>5</v>
       </c>
       <c r="C38">
-        <v>0.60769700000000004</v>
+        <v>0.63084499999999999</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
       </c>
       <c r="E38">
-        <v>0.212085</v>
+        <v>0.21190700000000001</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
       </c>
       <c r="G38">
-        <v>0.268899</v>
+        <v>0.273484</v>
       </c>
       <c r="H38" t="s">
         <v>14</v>
       </c>
       <c r="I38">
-        <v>0.18920300000000001</v>
+        <v>0.18907299999999999</v>
       </c>
       <c r="J38" t="s">
         <v>15</v>
@@ -13252,7 +13249,7 @@
         <v>17</v>
       </c>
       <c r="O38">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S38" s="4"/>
     </row>
@@ -13261,25 +13258,25 @@
         <v>5</v>
       </c>
       <c r="C39">
-        <v>0.59667599999999998</v>
+        <v>0.60798200000000002</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
       </c>
       <c r="E39">
-        <v>0.211896</v>
+        <v>0.21196599999999999</v>
       </c>
       <c r="F39" t="s">
         <v>13</v>
       </c>
       <c r="G39">
-        <v>0.263297</v>
+        <v>0.27032099999999998</v>
       </c>
       <c r="H39" t="s">
         <v>14</v>
       </c>
       <c r="I39">
-        <v>0.189196</v>
+        <v>0.18926299999999999</v>
       </c>
       <c r="J39" t="s">
         <v>15</v>
@@ -13297,7 +13294,7 @@
         <v>17</v>
       </c>
       <c r="O39">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S39" s="4"/>
     </row>
@@ -13306,25 +13303,25 @@
         <v>5</v>
       </c>
       <c r="C40">
-        <v>0.60183299999999995</v>
+        <v>0.60870800000000003</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
       </c>
       <c r="E40">
-        <v>0.21209700000000001</v>
+        <v>0.212038</v>
       </c>
       <c r="F40" t="s">
         <v>13</v>
       </c>
       <c r="G40">
-        <v>0.26583099999999998</v>
+        <v>0.26485399999999998</v>
       </c>
       <c r="H40" t="s">
         <v>14</v>
       </c>
       <c r="I40">
-        <v>0.189085</v>
+        <v>0.18920300000000001</v>
       </c>
       <c r="J40" t="s">
         <v>15</v>
@@ -13342,7 +13339,7 @@
         <v>17</v>
       </c>
       <c r="O40">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S40" s="4"/>
     </row>
@@ -13351,25 +13348,25 @@
         <v>5</v>
       </c>
       <c r="C41">
-        <v>0.61939500000000003</v>
+        <v>0.62415100000000001</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
       </c>
       <c r="E41">
-        <v>0.21160699999999999</v>
+        <v>0.21185300000000001</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
       </c>
       <c r="G41">
-        <v>0.26705400000000001</v>
+        <v>0.27186300000000002</v>
       </c>
       <c r="H41" t="s">
         <v>14</v>
       </c>
       <c r="I41">
-        <v>0.18912599999999999</v>
+        <v>0.189133</v>
       </c>
       <c r="J41" t="s">
         <v>15</v>
@@ -13387,7 +13384,7 @@
         <v>17</v>
       </c>
       <c r="O41">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S41" s="4"/>
     </row>
@@ -13396,25 +13393,25 @@
         <v>5</v>
       </c>
       <c r="C42">
-        <v>0.60159399999999996</v>
+        <v>0.62352799999999997</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
       <c r="E42">
-        <v>0.21163899999999999</v>
+        <v>0.21199200000000001</v>
       </c>
       <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42">
-        <v>0.26346999999999998</v>
+        <v>0.285271</v>
       </c>
       <c r="H42" t="s">
         <v>14</v>
       </c>
       <c r="I42">
-        <v>0.189196</v>
+        <v>0.18921299999999999</v>
       </c>
       <c r="J42" t="s">
         <v>15</v>
@@ -13432,7 +13429,7 @@
         <v>17</v>
       </c>
       <c r="O42">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S42" s="4"/>
     </row>
@@ -13441,25 +13438,25 @@
         <v>5</v>
       </c>
       <c r="C43">
-        <v>0.61033999999999999</v>
+        <v>0.61589300000000002</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
       </c>
       <c r="E43">
-        <v>0.212059</v>
+        <v>0.212202</v>
       </c>
       <c r="F43" t="s">
         <v>13</v>
       </c>
       <c r="G43">
-        <v>0.26763799999999999</v>
+        <v>0.273482</v>
       </c>
       <c r="H43" t="s">
         <v>14</v>
       </c>
       <c r="I43">
-        <v>0.189193</v>
+        <v>0.18924099999999999</v>
       </c>
       <c r="J43" t="s">
         <v>15</v>
@@ -13477,7 +13474,7 @@
         <v>17</v>
       </c>
       <c r="O43">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S43" s="4"/>
     </row>
@@ -13486,25 +13483,25 @@
         <v>5</v>
       </c>
       <c r="C44">
-        <v>0.60018800000000005</v>
+        <v>0.64928399999999997</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
       </c>
       <c r="E44">
-        <v>0.21207599999999999</v>
+        <v>0.212038</v>
       </c>
       <c r="F44" t="s">
         <v>13</v>
       </c>
       <c r="G44">
-        <v>0.26765099999999997</v>
+        <v>0.279223</v>
       </c>
       <c r="H44" t="s">
         <v>14</v>
       </c>
       <c r="I44">
-        <v>0.189245</v>
+        <v>0.189106</v>
       </c>
       <c r="J44" t="s">
         <v>15</v>
@@ -13522,7 +13519,7 @@
         <v>17</v>
       </c>
       <c r="O44">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S44" s="4"/>
     </row>
@@ -13531,25 +13528,25 @@
         <v>5</v>
       </c>
       <c r="C45">
-        <v>0.61316000000000004</v>
+        <v>0.63702300000000001</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
       </c>
       <c r="E45">
-        <v>0.212196</v>
+        <v>0.212198</v>
       </c>
       <c r="F45" t="s">
         <v>13</v>
       </c>
       <c r="G45">
-        <v>0.27172099999999999</v>
+        <v>0.279393</v>
       </c>
       <c r="H45" t="s">
         <v>14</v>
       </c>
       <c r="I45">
-        <v>0.18915000000000001</v>
+        <v>0.18915699999999999</v>
       </c>
       <c r="J45" t="s">
         <v>15</v>
@@ -13567,7 +13564,7 @@
         <v>17</v>
       </c>
       <c r="O45">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S45" s="4"/>
     </row>
@@ -13576,25 +13573,25 @@
         <v>5</v>
       </c>
       <c r="C46">
-        <v>0.59518300000000002</v>
+        <v>0.60484700000000002</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
       </c>
       <c r="E46">
-        <v>0.212036</v>
+        <v>0.212149</v>
       </c>
       <c r="F46" t="s">
         <v>13</v>
       </c>
       <c r="G46">
-        <v>0.26292599999999999</v>
+        <v>0.26269900000000002</v>
       </c>
       <c r="H46" t="s">
         <v>14</v>
       </c>
       <c r="I46">
-        <v>0.189253</v>
+        <v>0.18912200000000001</v>
       </c>
       <c r="J46" t="s">
         <v>15</v>
@@ -13612,7 +13609,7 @@
         <v>17</v>
       </c>
       <c r="O46">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S46" s="4"/>
     </row>
@@ -13621,25 +13618,25 @@
         <v>5</v>
       </c>
       <c r="C47">
-        <v>0.60369799999999996</v>
+        <v>0.62011300000000003</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
       </c>
       <c r="E47">
-        <v>0.21202699999999999</v>
+        <v>0.21199499999999999</v>
       </c>
       <c r="F47" t="s">
         <v>13</v>
       </c>
       <c r="G47">
-        <v>0.26538800000000001</v>
+        <v>0.26975199999999999</v>
       </c>
       <c r="H47" t="s">
         <v>14</v>
       </c>
       <c r="I47">
-        <v>0.18922600000000001</v>
+        <v>0.18926000000000001</v>
       </c>
       <c r="J47" t="s">
         <v>15</v>
@@ -13657,7 +13654,7 @@
         <v>17</v>
       </c>
       <c r="O47">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S47" s="4"/>
     </row>
@@ -13666,25 +13663,25 @@
         <v>5</v>
       </c>
       <c r="C48">
-        <v>0.60346599999999995</v>
+        <v>0.63824599999999998</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
       </c>
       <c r="E48">
-        <v>0.21201300000000001</v>
+        <v>0.21185699999999999</v>
       </c>
       <c r="F48" t="s">
         <v>13</v>
       </c>
       <c r="G48">
-        <v>0.26579900000000001</v>
+        <v>0.277721</v>
       </c>
       <c r="H48" t="s">
         <v>14</v>
       </c>
       <c r="I48">
-        <v>0.18917200000000001</v>
+        <v>0.18904000000000001</v>
       </c>
       <c r="J48" t="s">
         <v>15</v>
@@ -13702,7 +13699,7 @@
         <v>17</v>
       </c>
       <c r="O48">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S48" s="4"/>
     </row>
@@ -13711,25 +13708,25 @@
         <v>5</v>
       </c>
       <c r="C49">
-        <v>0.60217500000000002</v>
+        <v>0.63867099999999999</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
       </c>
       <c r="E49">
-        <v>0.211951</v>
+        <v>0.21199699999999999</v>
       </c>
       <c r="F49" t="s">
         <v>13</v>
       </c>
       <c r="G49">
-        <v>0.26638600000000001</v>
+        <v>0.29538199999999998</v>
       </c>
       <c r="H49" t="s">
         <v>14</v>
       </c>
       <c r="I49">
-        <v>0.18912499999999999</v>
+        <v>0.18915299999999999</v>
       </c>
       <c r="J49" t="s">
         <v>15</v>
@@ -13747,7 +13744,7 @@
         <v>17</v>
       </c>
       <c r="O49">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S49" s="4"/>
     </row>
@@ -13756,25 +13753,25 @@
         <v>5</v>
       </c>
       <c r="C50">
-        <v>0.61191200000000001</v>
+        <v>0.63412100000000005</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50">
-        <v>0.21185599999999999</v>
+        <v>0.212366</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>
       </c>
       <c r="G50">
-        <v>0.27393000000000001</v>
+        <v>0.27136199999999999</v>
       </c>
       <c r="H50" t="s">
         <v>14</v>
       </c>
       <c r="I50">
-        <v>0.18915999999999999</v>
+        <v>0.189133</v>
       </c>
       <c r="J50" t="s">
         <v>15</v>
@@ -13792,7 +13789,7 @@
         <v>17</v>
       </c>
       <c r="O50">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S50" s="4"/>
     </row>
@@ -13801,25 +13798,25 @@
         <v>5</v>
       </c>
       <c r="C51">
-        <v>0.607298</v>
+        <v>0.62042399999999998</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51">
-        <v>0.21198600000000001</v>
+        <v>0.212232</v>
       </c>
       <c r="F51" t="s">
         <v>13</v>
       </c>
       <c r="G51">
-        <v>0.26543899999999998</v>
+        <v>0.268926</v>
       </c>
       <c r="H51" t="s">
         <v>14</v>
       </c>
       <c r="I51">
-        <v>0.189138</v>
+        <v>0.18914300000000001</v>
       </c>
       <c r="J51" t="s">
         <v>15</v>
@@ -13837,7 +13834,7 @@
         <v>17</v>
       </c>
       <c r="O51">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S51" s="4"/>
     </row>
@@ -13846,25 +13843,25 @@
         <v>5</v>
       </c>
       <c r="C52">
-        <v>0.60635099999999997</v>
+        <v>0.63208500000000001</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52">
-        <v>0.21207000000000001</v>
+        <v>0.21224999999999999</v>
       </c>
       <c r="F52" t="s">
         <v>13</v>
       </c>
       <c r="G52">
-        <v>0.26782699999999998</v>
+        <v>0.29220400000000002</v>
       </c>
       <c r="H52" t="s">
         <v>14</v>
       </c>
       <c r="I52">
-        <v>0.18910099999999999</v>
+        <v>0.18919</v>
       </c>
       <c r="J52" t="s">
         <v>15</v>
@@ -13882,7 +13879,7 @@
         <v>17</v>
       </c>
       <c r="O52">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S52" s="4"/>
     </row>
@@ -13891,25 +13888,25 @@
         <v>5</v>
       </c>
       <c r="C53">
-        <v>0.60377899999999995</v>
+        <v>0.64890599999999998</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
       </c>
       <c r="E53">
-        <v>0.212311</v>
+        <v>0.21166699999999999</v>
       </c>
       <c r="F53" t="s">
         <v>13</v>
       </c>
       <c r="G53">
-        <v>0.26393699999999998</v>
+        <v>0.280754</v>
       </c>
       <c r="H53" t="s">
         <v>14</v>
       </c>
       <c r="I53">
-        <v>0.18912000000000001</v>
+        <v>0.18913099999999999</v>
       </c>
       <c r="J53" t="s">
         <v>15</v>
@@ -13927,7 +13924,7 @@
         <v>17</v>
       </c>
       <c r="O53">
-        <v>10.154999999999999</v>
+        <v>10.558999999999999</v>
       </c>
       <c r="S53" s="4"/>
     </row>
@@ -13941,22 +13938,22 @@
       <c r="B55" s="5"/>
       <c r="C55" s="6">
         <f>AVERAGE(C3:C53)</f>
-        <v>0.54638452745098043</v>
+        <v>0.55957542156862727</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6">
         <f>AVERAGE(E3:E53)</f>
-        <v>0.19987980941176473</v>
+        <v>0.19986381490196076</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6">
         <f>AVERAGE(G3:G53)</f>
-        <v>0.22660652156862748</v>
+        <v>0.23333779803921564</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="6">
         <f>AVERAGE(I3:I53)</f>
-        <v>0.16108125470588239</v>
+        <v>0.16105950470588234</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6">
@@ -13971,7 +13968,7 @@
       <c r="N55" s="6"/>
       <c r="O55" s="6">
         <f>AVERAGE(O3:O53)</f>
-        <v>9.5349999999999877</v>
+        <v>9.9235686274509938</v>
       </c>
       <c r="P55" s="6"/>
       <c r="Q55" s="6"/>

</xml_diff>